<commit_message>
sumo archivos de prueba para la db.
</commit_message>
<xml_diff>
--- a/base.xlsx
+++ b/base.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" tabRatio="784"/>
   </bookViews>
   <sheets>
     <sheet name="servicio" sheetId="1" r:id="rId1"/>
@@ -18,15 +18,18 @@
     <sheet name="sitio" sheetId="12" r:id="rId9"/>
     <sheet name="favoritos" sheetId="10" r:id="rId10"/>
     <sheet name="administrador" sheetId="4" r:id="rId11"/>
-    <sheet name="cobranza" sheetId="8" r:id="rId12"/>
-    <sheet name="cuentaCorriente" sheetId="9" r:id="rId13"/>
+    <sheet name="zona" sheetId="15" r:id="rId12"/>
+    <sheet name="cobertura" sheetId="14" r:id="rId13"/>
+    <sheet name="contrato" sheetId="16" r:id="rId14"/>
+    <sheet name="cobranza" sheetId="8" r:id="rId15"/>
+    <sheet name="cuentaCorriente" sheetId="9" r:id="rId16"/>
   </sheets>
   <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="94">
   <si>
     <t>Electricidad</t>
   </si>
@@ -199,12 +202,6 @@
     <t>categoria</t>
   </si>
   <si>
-    <t>proMas</t>
-  </si>
-  <si>
-    <t>proFem</t>
-  </si>
-  <si>
     <t>nombre</t>
   </si>
   <si>
@@ -305,6 +302,15 @@
   </si>
   <si>
     <t>resultadoUser</t>
+  </si>
+  <si>
+    <t>servicio_id</t>
+  </si>
+  <si>
+    <t>pro_mas</t>
+  </si>
+  <si>
+    <t>pro_fem</t>
   </si>
 </sst>
 </file>
@@ -649,7 +655,7 @@
   <dimension ref="A1:K23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O10" sqref="O10"/>
+      <selection activeCell="M25" sqref="M25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -665,7 +671,7 @@
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>54</v>
+        <v>91</v>
       </c>
       <c r="B1" t="s">
         <v>55</v>
@@ -674,28 +680,28 @@
         <v>56</v>
       </c>
       <c r="D1" t="s">
-        <v>57</v>
+        <v>92</v>
       </c>
       <c r="E1" t="s">
-        <v>58</v>
+        <v>93</v>
       </c>
       <c r="F1" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="G1" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="H1" t="s">
+        <v>63</v>
+      </c>
+      <c r="I1" t="s">
+        <v>64</v>
+      </c>
+      <c r="J1" t="s">
+        <v>66</v>
+      </c>
+      <c r="K1" t="s">
         <v>65</v>
-      </c>
-      <c r="I1" t="s">
-        <v>66</v>
-      </c>
-      <c r="J1" t="s">
-        <v>68</v>
-      </c>
-      <c r="K1" t="s">
-        <v>67</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
@@ -1051,9 +1057,37 @@
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D1" sqref="D1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>54</v>
+      </c>
+      <c r="B1" t="s">
+        <v>57</v>
+      </c>
+      <c r="C1" t="s">
+        <v>72</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="R32" sqref="R32"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
@@ -1061,12 +1095,36 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="L1" sqref="L1:O1"/>
+      <selection activeCell="K10" sqref="K10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1076,46 +1134,46 @@
         <v>54</v>
       </c>
       <c r="B1" t="s">
+        <v>57</v>
+      </c>
+      <c r="C1" t="s">
+        <v>58</v>
+      </c>
+      <c r="D1" t="s">
         <v>59</v>
       </c>
-      <c r="C1" t="s">
+      <c r="E1" t="s">
         <v>60</v>
       </c>
-      <c r="D1" t="s">
+      <c r="F1" t="s">
         <v>61</v>
       </c>
-      <c r="E1" t="s">
+      <c r="G1" t="s">
         <v>62</v>
       </c>
-      <c r="F1" t="s">
+      <c r="H1" t="s">
+        <v>68</v>
+      </c>
+      <c r="I1" t="s">
+        <v>69</v>
+      </c>
+      <c r="J1" t="s">
+        <v>70</v>
+      </c>
+      <c r="K1" t="s">
+        <v>67</v>
+      </c>
+      <c r="L1" t="s">
         <v>63</v>
       </c>
-      <c r="G1" t="s">
+      <c r="M1" t="s">
         <v>64</v>
       </c>
-      <c r="H1" t="s">
-        <v>70</v>
-      </c>
-      <c r="I1" t="s">
-        <v>71</v>
-      </c>
-      <c r="J1" t="s">
-        <v>72</v>
-      </c>
-      <c r="K1" t="s">
-        <v>69</v>
-      </c>
-      <c r="L1" t="s">
+      <c r="N1" t="s">
+        <v>66</v>
+      </c>
+      <c r="O1" t="s">
         <v>65</v>
-      </c>
-      <c r="M1" t="s">
-        <v>66</v>
-      </c>
-      <c r="N1" t="s">
-        <v>68</v>
-      </c>
-      <c r="O1" t="s">
-        <v>67</v>
       </c>
     </row>
   </sheetData>
@@ -1139,58 +1197,58 @@
         <v>54</v>
       </c>
       <c r="B1" t="s">
+        <v>73</v>
+      </c>
+      <c r="C1" t="s">
+        <v>57</v>
+      </c>
+      <c r="D1" t="s">
+        <v>67</v>
+      </c>
+      <c r="E1" t="s">
+        <v>74</v>
+      </c>
+      <c r="F1" t="s">
         <v>75</v>
       </c>
-      <c r="C1" t="s">
-        <v>59</v>
-      </c>
-      <c r="D1" t="s">
-        <v>69</v>
-      </c>
-      <c r="E1" t="s">
+      <c r="G1" t="s">
+        <v>60</v>
+      </c>
+      <c r="H1" t="s">
+        <v>72</v>
+      </c>
+      <c r="I1" t="s">
+        <v>62</v>
+      </c>
+      <c r="J1" t="s">
+        <v>68</v>
+      </c>
+      <c r="K1" t="s">
         <v>76</v>
       </c>
-      <c r="F1" t="s">
+      <c r="L1" t="s">
+        <v>70</v>
+      </c>
+      <c r="M1" t="s">
         <v>77</v>
       </c>
-      <c r="G1" t="s">
-        <v>62</v>
-      </c>
-      <c r="H1" t="s">
-        <v>74</v>
-      </c>
-      <c r="I1" t="s">
+      <c r="N1" t="s">
+        <v>78</v>
+      </c>
+      <c r="O1" t="s">
+        <v>79</v>
+      </c>
+      <c r="P1" t="s">
+        <v>63</v>
+      </c>
+      <c r="Q1" t="s">
         <v>64</v>
       </c>
-      <c r="J1" t="s">
-        <v>70</v>
-      </c>
-      <c r="K1" t="s">
-        <v>78</v>
-      </c>
-      <c r="L1" t="s">
-        <v>72</v>
-      </c>
-      <c r="M1" t="s">
-        <v>79</v>
-      </c>
-      <c r="N1" t="s">
-        <v>80</v>
-      </c>
-      <c r="O1" t="s">
-        <v>81</v>
-      </c>
-      <c r="P1" t="s">
+      <c r="R1" t="s">
+        <v>66</v>
+      </c>
+      <c r="S1" t="s">
         <v>65</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>66</v>
-      </c>
-      <c r="R1" t="s">
-        <v>68</v>
-      </c>
-      <c r="S1" t="s">
-        <v>67</v>
       </c>
     </row>
   </sheetData>
@@ -1216,37 +1274,37 @@
         <v>54</v>
       </c>
       <c r="B1" t="s">
+        <v>80</v>
+      </c>
+      <c r="C1" t="s">
+        <v>73</v>
+      </c>
+      <c r="D1" t="s">
+        <v>81</v>
+      </c>
+      <c r="E1" t="s">
+        <v>70</v>
+      </c>
+      <c r="F1" t="s">
         <v>82</v>
       </c>
-      <c r="C1" t="s">
-        <v>75</v>
-      </c>
-      <c r="D1" t="s">
+      <c r="G1" t="s">
         <v>83</v>
       </c>
-      <c r="E1" t="s">
-        <v>72</v>
-      </c>
-      <c r="F1" t="s">
+      <c r="H1" t="s">
         <v>84</v>
       </c>
-      <c r="G1" t="s">
-        <v>85</v>
-      </c>
-      <c r="H1" t="s">
-        <v>86</v>
-      </c>
       <c r="I1" t="s">
+        <v>63</v>
+      </c>
+      <c r="J1" t="s">
+        <v>64</v>
+      </c>
+      <c r="K1" t="s">
+        <v>66</v>
+      </c>
+      <c r="L1" t="s">
         <v>65</v>
-      </c>
-      <c r="J1" t="s">
-        <v>66</v>
-      </c>
-      <c r="K1" t="s">
-        <v>68</v>
-      </c>
-      <c r="L1" t="s">
-        <v>67</v>
       </c>
     </row>
   </sheetData>
@@ -1274,22 +1332,22 @@
         <v>54</v>
       </c>
       <c r="B1" t="s">
+        <v>85</v>
+      </c>
+      <c r="C1" t="s">
         <v>87</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
+        <v>86</v>
+      </c>
+      <c r="E1" t="s">
+        <v>88</v>
+      </c>
+      <c r="F1" t="s">
         <v>89</v>
       </c>
-      <c r="D1" t="s">
-        <v>88</v>
-      </c>
-      <c r="E1" t="s">
+      <c r="G1" t="s">
         <v>90</v>
-      </c>
-      <c r="F1" t="s">
-        <v>91</v>
-      </c>
-      <c r="G1" t="s">
-        <v>92</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
upgrade del AS y grandle a 3.4 y 5.$.
</commit_message>
<xml_diff>
--- a/base.xlsx
+++ b/base.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" tabRatio="784"/>
@@ -316,8 +316,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -408,7 +408,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -440,10 +440,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -475,7 +474,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -651,14 +649,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:K23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M25" sqref="M25"/>
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
     <col min="2" max="2" width="12.42578125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="21" bestFit="1" customWidth="1"/>
@@ -669,7 +667,7 @@
     <col min="9" max="9" width="11.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11">
       <c r="A1" t="s">
         <v>91</v>
       </c>
@@ -704,7 +702,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11">
       <c r="B2" t="s">
         <v>20</v>
       </c>
@@ -718,7 +716,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11">
       <c r="B3" t="s">
         <v>20</v>
       </c>
@@ -732,7 +730,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11">
       <c r="B4" t="s">
         <v>20</v>
       </c>
@@ -746,7 +744,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11">
       <c r="B5" t="s">
         <v>21</v>
       </c>
@@ -760,7 +758,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11">
       <c r="B6" t="s">
         <v>21</v>
       </c>
@@ -774,7 +772,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11">
       <c r="B7" t="s">
         <v>22</v>
       </c>
@@ -788,7 +786,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11">
       <c r="B8" t="s">
         <v>23</v>
       </c>
@@ -802,7 +800,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11">
       <c r="B9" t="s">
         <v>23</v>
       </c>
@@ -816,7 +814,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11">
       <c r="B10" t="s">
         <v>24</v>
       </c>
@@ -830,7 +828,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11">
       <c r="B11" t="s">
         <v>25</v>
       </c>
@@ -844,7 +842,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11">
       <c r="B12" t="s">
         <v>26</v>
       </c>
@@ -858,7 +856,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11">
       <c r="B13" t="s">
         <v>27</v>
       </c>
@@ -872,7 +870,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11">
       <c r="B14" t="s">
         <v>27</v>
       </c>
@@ -886,7 +884,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11">
       <c r="B15" t="s">
         <v>27</v>
       </c>
@@ -900,7 +898,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11">
       <c r="B16" t="s">
         <v>27</v>
       </c>
@@ -914,7 +912,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="17" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:5">
       <c r="B17" t="s">
         <v>27</v>
       </c>
@@ -928,7 +926,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="18" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:5">
       <c r="B18" t="s">
         <v>28</v>
       </c>
@@ -942,7 +940,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="19" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:5">
       <c r="B19" t="s">
         <v>28</v>
       </c>
@@ -956,7 +954,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="20" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:5">
       <c r="B20" t="s">
         <v>28</v>
       </c>
@@ -970,7 +968,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="21" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:5">
       <c r="B21" t="s">
         <v>28</v>
       </c>
@@ -984,7 +982,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="22" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:5">
       <c r="B22" t="s">
         <v>28</v>
       </c>
@@ -998,7 +996,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="23" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:5">
       <c r="B23" t="s">
         <v>28</v>
       </c>
@@ -1018,54 +1016,54 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="K34" sqref="K34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3">
       <c r="A1" t="s">
         <v>54</v>
       </c>
@@ -1082,54 +1080,54 @@
 </file>
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="R32" sqref="R32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:O1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="K10" sqref="K10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15">
       <c r="A1" t="s">
         <v>54</v>
       </c>
@@ -1183,16 +1181,16 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:S1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="P1" sqref="P1:S1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:19">
       <c r="A1" t="s">
         <v>54</v>
       </c>
@@ -1257,19 +1255,19 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:L1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="I1" sqref="I1:L1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
     <col min="8" max="8" width="11.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12">
       <c r="A1" t="s">
         <v>54</v>
       </c>
@@ -1313,21 +1311,21 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:G1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="H1" sqref="H1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="10.85546875" customWidth="1"/>
     <col min="6" max="6" width="12.42578125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="13.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7">
       <c r="A1" t="s">
         <v>54</v>
       </c>
@@ -1356,48 +1354,48 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>